<commit_message>
cigna close changes done
</commit_message>
<xml_diff>
--- a/Input/Cigna_Close_Care/benefits.xlsx
+++ b/Input/Cigna_Close_Care/benefits.xlsx
@@ -571,7 +571,7 @@
         <v>USD 500,000</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>Worldwide including USA/Worldwide excluding USA</v>
+        <v>Worldwide excluding USA</v>
       </c>
       <c r="D2" s="1" t="str">
         <v>Inhouse Network</v>
@@ -692,7 +692,7 @@
         <v>Annually</v>
       </c>
       <c r="AQ2" s="1" t="str">
-        <v>Worldwide including USA</v>
+        <v>Worldwide excluding USA</v>
       </c>
       <c r="AR2" s="1" t="str">
         <v>Dental</v>
@@ -728,9 +728,6 @@
       </c>
       <c r="AL3" s="1" t="str">
         <v>$0, 10% Co-insurance, $3,000 Out of pocket</v>
-      </c>
-      <c r="AQ3" s="1" t="str">
-        <v>Worldwide excluding USA</v>
       </c>
       <c r="AY3" s="1" t="str">
         <v>OP</v>

</xml_diff>